<commit_message>
updated files with duplicate site coords
</commit_message>
<xml_diff>
--- a/ISRaD_Data/Masiello_2004.xlsx
+++ b/ISRaD_Data/Masiello_2004.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="28705"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="660" windowWidth="24560" windowHeight="8260" activeTab="6"/>
+    <workbookView xWindow="120" yWindow="660" windowWidth="18980" windowHeight="15300" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="metadata" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
     <sheet name="incubation" sheetId="8" r:id="rId8"/>
     <sheet name="controlled vocabulary" sheetId="9" r:id="rId9"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2297" uniqueCount="1360">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2306" uniqueCount="1362">
   <si>
     <t>entry_name</t>
   </si>
@@ -4109,13 +4109,19 @@
   </si>
   <si>
     <t>frc_fraction_modern_sd</t>
+  </si>
+  <si>
+    <t>Mattole</t>
+  </si>
+  <si>
+    <t>pro_elevation</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -4135,6 +4141,22 @@
       <color rgb="FF000000"/>
       <name val="Tahoma"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -4188,8 +4210,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4203,7 +4239,21 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="15">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4695,9 +4745,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G4" sqref="G4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" t="s">
@@ -4894,13 +4949,20 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AJ10"/>
+  <dimension ref="A1:AK10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="2" max="2" width="18.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:36">
+    <row r="1" spans="1:37">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -4923,94 +4985,97 @@
         <v>89</v>
       </c>
       <c r="H1" t="s">
+        <v>1361</v>
+      </c>
+      <c r="I1" t="s">
         <v>90</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>91</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>92</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>93</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>94</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>95</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>96</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>97</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>98</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>99</v>
       </c>
-      <c r="R1" t="s">
+      <c r="S1" t="s">
         <v>100</v>
       </c>
-      <c r="S1" t="s">
+      <c r="T1" t="s">
         <v>101</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>102</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>103</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>104</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>105</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Y1" t="s">
         <v>106</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="Z1" t="s">
         <v>107</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AA1" t="s">
         <v>108</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AB1" t="s">
         <v>109</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AC1" t="s">
         <v>110</v>
       </c>
-      <c r="AC1" t="s">
+      <c r="AD1" t="s">
         <v>111</v>
       </c>
-      <c r="AD1" t="s">
+      <c r="AE1" t="s">
         <v>112</v>
       </c>
-      <c r="AE1" t="s">
+      <c r="AF1" t="s">
         <v>113</v>
       </c>
-      <c r="AF1" t="s">
+      <c r="AG1" t="s">
         <v>114</v>
       </c>
-      <c r="AG1" t="s">
+      <c r="AH1" t="s">
         <v>115</v>
       </c>
-      <c r="AH1" t="s">
+      <c r="AI1" t="s">
         <v>116</v>
       </c>
-      <c r="AI1" t="s">
+      <c r="AJ1" t="s">
         <v>117</v>
       </c>
-      <c r="AJ1" t="s">
+      <c r="AK1" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="2" spans="1:36">
+    <row r="2" spans="1:37">
       <c r="A2" t="s">
         <v>16</v>
       </c>
@@ -5032,95 +5097,95 @@
       <c r="G2" t="s">
         <v>63</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>122</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>123</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>124</v>
       </c>
-      <c r="K2" t="s">
+      <c r="L2" t="s">
         <v>125</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
         <v>126</v>
       </c>
-      <c r="M2" t="s">
+      <c r="N2" t="s">
         <v>127</v>
       </c>
-      <c r="N2" t="s">
+      <c r="O2" t="s">
         <v>128</v>
       </c>
-      <c r="O2" t="s">
+      <c r="P2" t="s">
         <v>129</v>
       </c>
-      <c r="P2" t="s">
+      <c r="Q2" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>131</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>132</v>
       </c>
-      <c r="S2" t="s">
+      <c r="T2" t="s">
         <v>133</v>
       </c>
-      <c r="T2" t="s">
+      <c r="U2" t="s">
         <v>134</v>
       </c>
-      <c r="U2" t="s">
+      <c r="V2" t="s">
         <v>135</v>
       </c>
-      <c r="V2" t="s">
+      <c r="W2" t="s">
         <v>136</v>
       </c>
-      <c r="W2" t="s">
+      <c r="X2" t="s">
         <v>137</v>
       </c>
-      <c r="X2" t="s">
+      <c r="Y2" t="s">
         <v>138</v>
       </c>
-      <c r="Y2" t="s">
+      <c r="Z2" t="s">
         <v>139</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>140</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>141</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>142</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AD2" t="s">
         <v>143</v>
       </c>
-      <c r="AD2" t="s">
+      <c r="AE2" t="s">
         <v>144</v>
       </c>
-      <c r="AE2" t="s">
+      <c r="AF2" t="s">
         <v>145</v>
       </c>
-      <c r="AF2" t="s">
+      <c r="AG2" t="s">
         <v>146</v>
       </c>
-      <c r="AG2" t="s">
+      <c r="AH2" t="s">
         <v>147</v>
       </c>
-      <c r="AH2" t="s">
+      <c r="AI2" t="s">
         <v>148</v>
       </c>
-      <c r="AI2" t="s">
+      <c r="AJ2" t="s">
         <v>149</v>
       </c>
-      <c r="AJ2" t="s">
+      <c r="AK2" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="3" spans="1:36">
+    <row r="3" spans="1:37">
       <c r="A3" t="s">
         <v>31</v>
       </c>
@@ -5134,43 +5199,43 @@
         <v>67</v>
       </c>
       <c r="H3" t="s">
+        <v>69</v>
+      </c>
+      <c r="I3" t="s">
         <v>152</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>153</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>154</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>155</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>36</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>156</v>
       </c>
-      <c r="P3" t="s">
+      <c r="Q3" t="s">
         <v>157</v>
       </c>
-      <c r="Q3" t="s">
+      <c r="R3" t="s">
         <v>158</v>
       </c>
-      <c r="R3" t="s">
+      <c r="S3" t="s">
         <v>155</v>
       </c>
-      <c r="S3" t="s">
+      <c r="T3" t="s">
         <v>159</v>
       </c>
-      <c r="T3" t="s">
+      <c r="U3" t="s">
         <v>160</v>
       </c>
-      <c r="U3" t="s">
+      <c r="V3" t="s">
         <v>161</v>
-      </c>
-      <c r="V3" t="s">
-        <v>162</v>
       </c>
       <c r="W3" t="s">
         <v>162</v>
@@ -5179,326 +5244,350 @@
         <v>162</v>
       </c>
       <c r="Y3" t="s">
+        <v>162</v>
+      </c>
+      <c r="Z3" t="s">
         <v>163</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>164</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>165</v>
       </c>
-      <c r="AB3" t="s">
+      <c r="AC3" t="s">
         <v>166</v>
       </c>
-      <c r="AC3" t="s">
+      <c r="AD3" t="s">
         <v>167</v>
       </c>
-      <c r="AD3" t="s">
+      <c r="AE3" t="s">
         <v>168</v>
       </c>
-      <c r="AE3" t="s">
+      <c r="AF3" t="s">
         <v>159</v>
       </c>
-      <c r="AF3" t="s">
+      <c r="AG3" t="s">
         <v>169</v>
       </c>
-      <c r="AG3" t="s">
+      <c r="AH3" t="s">
         <v>170</v>
-      </c>
-      <c r="AH3" t="s">
-        <v>171</v>
       </c>
       <c r="AI3" t="s">
         <v>171</v>
       </c>
       <c r="AJ3" t="s">
+        <v>171</v>
+      </c>
+      <c r="AK3" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="4" spans="1:36">
+    <row r="4" spans="1:37">
       <c r="A4" t="s">
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="D4" t="s">
         <v>172</v>
       </c>
       <c r="H4" t="s">
+        <v>73</v>
+      </c>
+      <c r="I4" t="s">
         <v>173</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>174</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>175</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>176</v>
       </c>
-      <c r="P4" t="s">
+      <c r="Q4" t="s">
         <v>177</v>
       </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>178</v>
       </c>
-      <c r="T4" t="s">
+      <c r="U4" t="s">
         <v>179</v>
       </c>
-      <c r="U4" t="s">
+      <c r="V4" t="s">
         <v>180</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>181</v>
       </c>
-      <c r="AE4" t="s">
+      <c r="AF4" t="s">
         <v>182</v>
       </c>
     </row>
-    <row r="5" spans="1:36">
+    <row r="5" spans="1:37">
       <c r="A5" t="s">
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="D5" t="s">
         <v>183</v>
       </c>
       <c r="H5" t="s">
+        <v>75</v>
+      </c>
+      <c r="I5" t="s">
         <v>173</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>174</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>175</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>184</v>
       </c>
-      <c r="P5" t="s">
+      <c r="Q5" t="s">
         <v>177</v>
       </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>84</v>
       </c>
-      <c r="T5" t="s">
+      <c r="U5" t="s">
         <v>179</v>
       </c>
-      <c r="U5" t="s">
+      <c r="V5" t="s">
         <v>180</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>181</v>
       </c>
-      <c r="AE5" t="s">
+      <c r="AF5" t="s">
         <v>185</v>
       </c>
     </row>
-    <row r="6" spans="1:36">
+    <row r="6" spans="1:37">
       <c r="A6" t="s">
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="D6" t="s">
         <v>186</v>
       </c>
       <c r="H6" t="s">
+        <v>77</v>
+      </c>
+      <c r="I6" t="s">
         <v>173</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>174</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>175</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>176</v>
       </c>
-      <c r="P6" t="s">
+      <c r="Q6" t="s">
         <v>177</v>
       </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>187</v>
       </c>
-      <c r="T6" t="s">
+      <c r="U6" t="s">
         <v>179</v>
       </c>
-      <c r="U6" t="s">
+      <c r="V6" t="s">
         <v>180</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>181</v>
       </c>
-      <c r="AE6" t="s">
+      <c r="AF6" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="7" spans="1:36">
+    <row r="7" spans="1:37">
       <c r="A7" t="s">
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="D7" t="s">
         <v>189</v>
       </c>
       <c r="H7" t="s">
+        <v>79</v>
+      </c>
+      <c r="I7" t="s">
         <v>173</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>174</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>175</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>184</v>
       </c>
-      <c r="P7" t="s">
+      <c r="Q7" t="s">
         <v>177</v>
       </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>190</v>
       </c>
-      <c r="T7" t="s">
+      <c r="U7" t="s">
         <v>179</v>
       </c>
-      <c r="U7" t="s">
+      <c r="V7" t="s">
         <v>180</v>
       </c>
-      <c r="AA7" t="s">
+      <c r="AB7" t="s">
         <v>181</v>
       </c>
-      <c r="AE7" t="s">
+      <c r="AF7" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="8" spans="1:36">
+    <row r="8" spans="1:37">
       <c r="A8" t="s">
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="D8" t="s">
         <v>191</v>
       </c>
       <c r="H8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
         <v>173</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>174</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>175</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>192</v>
       </c>
-      <c r="P8" t="s">
+      <c r="Q8" t="s">
         <v>177</v>
       </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>193</v>
       </c>
-      <c r="T8" t="s">
+      <c r="U8" t="s">
         <v>179</v>
       </c>
-      <c r="U8" t="s">
+      <c r="V8" t="s">
         <v>180</v>
       </c>
-      <c r="AA8" t="s">
+      <c r="AB8" t="s">
         <v>181</v>
       </c>
-      <c r="AE8" t="s">
+      <c r="AF8" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="9" spans="1:36">
+    <row r="9" spans="1:37">
       <c r="A9" t="s">
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="D9" t="s">
         <v>194</v>
       </c>
       <c r="H9" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" t="s">
         <v>173</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>174</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>175</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>184</v>
       </c>
-      <c r="P9" t="s">
+      <c r="Q9" t="s">
         <v>177</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>190</v>
       </c>
-      <c r="T9" t="s">
+      <c r="U9" t="s">
         <v>179</v>
       </c>
-      <c r="U9" t="s">
+      <c r="V9" t="s">
         <v>180</v>
       </c>
-      <c r="AA9" t="s">
+      <c r="AB9" t="s">
         <v>181</v>
       </c>
-      <c r="AE9" t="s">
+      <c r="AF9" t="s">
         <v>188</v>
       </c>
     </row>
-    <row r="10" spans="1:36">
+    <row r="10" spans="1:37">
       <c r="A10" t="s">
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="D10" t="s">
         <v>195</v>
       </c>
       <c r="H10" t="s">
+        <v>84</v>
+      </c>
+      <c r="I10" t="s">
         <v>173</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>174</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>175</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>192</v>
       </c>
-      <c r="P10" t="s">
+      <c r="Q10" t="s">
         <v>177</v>
       </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>196</v>
       </c>
-      <c r="T10" t="s">
+      <c r="U10" t="s">
         <v>179</v>
       </c>
-      <c r="U10" t="s">
+      <c r="V10" t="s">
         <v>180</v>
       </c>
-      <c r="AA10" t="s">
+      <c r="AB10" t="s">
         <v>181</v>
       </c>
-      <c r="AE10" t="s">
+      <c r="AF10" t="s">
         <v>197</v>
       </c>
     </row>
@@ -5839,14 +5928,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:CT59"/>
   <sheetViews>
-    <sheetView topLeftCell="AJ49" workbookViewId="0">
-      <selection activeCell="AV52" sqref="AV52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
+    <col min="1" max="1" width="16.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="23.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="22.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:98">
@@ -6685,7 +6776,7 @@
         <v>43</v>
       </c>
       <c r="B4" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C4" t="s">
         <v>191</v>
@@ -6744,7 +6835,7 @@
         <v>43</v>
       </c>
       <c r="B5" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C5" t="s">
         <v>191</v>
@@ -6803,7 +6894,7 @@
         <v>43</v>
       </c>
       <c r="B6" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C6" t="s">
         <v>191</v>
@@ -6862,7 +6953,7 @@
         <v>43</v>
       </c>
       <c r="B7" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C7" t="s">
         <v>191</v>
@@ -6921,7 +7012,7 @@
         <v>43</v>
       </c>
       <c r="B8" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C8" t="s">
         <v>191</v>
@@ -6980,7 +7071,7 @@
         <v>43</v>
       </c>
       <c r="B9" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C9" t="s">
         <v>191</v>
@@ -7039,7 +7130,7 @@
         <v>43</v>
       </c>
       <c r="B10" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C10" t="s">
         <v>191</v>
@@ -7098,7 +7189,7 @@
         <v>43</v>
       </c>
       <c r="B11" t="s">
-        <v>80</v>
+        <v>1360</v>
       </c>
       <c r="C11" t="s">
         <v>191</v>
@@ -7157,7 +7248,7 @@
         <v>43</v>
       </c>
       <c r="B12" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C12" t="s">
         <v>195</v>
@@ -7198,7 +7289,7 @@
         <v>43</v>
       </c>
       <c r="B13" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C13" t="s">
         <v>195</v>
@@ -7239,7 +7330,7 @@
         <v>43</v>
       </c>
       <c r="B14" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C14" t="s">
         <v>195</v>
@@ -7280,7 +7371,7 @@
         <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C15" t="s">
         <v>195</v>
@@ -7321,7 +7412,7 @@
         <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C16" t="s">
         <v>195</v>
@@ -7362,7 +7453,7 @@
         <v>43</v>
       </c>
       <c r="B17" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C17" t="s">
         <v>195</v>
@@ -7403,7 +7494,7 @@
         <v>43</v>
       </c>
       <c r="B18" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C18" t="s">
         <v>195</v>
@@ -7444,7 +7535,7 @@
         <v>43</v>
       </c>
       <c r="B19" t="s">
-        <v>83</v>
+        <v>1360</v>
       </c>
       <c r="C19" t="s">
         <v>195</v>
@@ -7485,7 +7576,7 @@
         <v>43</v>
       </c>
       <c r="B20" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C20" t="s">
         <v>194</v>
@@ -7544,7 +7635,7 @@
         <v>43</v>
       </c>
       <c r="B21" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C21" t="s">
         <v>194</v>
@@ -7603,7 +7694,7 @@
         <v>43</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C22" t="s">
         <v>194</v>
@@ -7662,7 +7753,7 @@
         <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C23" t="s">
         <v>194</v>
@@ -7721,7 +7812,7 @@
         <v>43</v>
       </c>
       <c r="B24" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C24" t="s">
         <v>194</v>
@@ -7780,7 +7871,7 @@
         <v>43</v>
       </c>
       <c r="B25" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C25" t="s">
         <v>194</v>
@@ -7839,7 +7930,7 @@
         <v>43</v>
       </c>
       <c r="B26" t="s">
-        <v>82</v>
+        <v>1360</v>
       </c>
       <c r="C26" t="s">
         <v>194</v>
@@ -7898,7 +7989,7 @@
         <v>43</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C27" t="s">
         <v>189</v>
@@ -7957,7 +8048,7 @@
         <v>43</v>
       </c>
       <c r="B28" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C28" t="s">
         <v>189</v>
@@ -8016,7 +8107,7 @@
         <v>43</v>
       </c>
       <c r="B29" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C29" t="s">
         <v>189</v>
@@ -8075,7 +8166,7 @@
         <v>43</v>
       </c>
       <c r="B30" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C30" t="s">
         <v>189</v>
@@ -8134,7 +8225,7 @@
         <v>43</v>
       </c>
       <c r="B31" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C31" t="s">
         <v>189</v>
@@ -8193,7 +8284,7 @@
         <v>43</v>
       </c>
       <c r="B32" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C32" t="s">
         <v>189</v>
@@ -8252,7 +8343,7 @@
         <v>43</v>
       </c>
       <c r="B33" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C33" t="s">
         <v>189</v>
@@ -8311,7 +8402,7 @@
         <v>43</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C34" t="s">
         <v>189</v>
@@ -8370,7 +8461,7 @@
         <v>43</v>
       </c>
       <c r="B35" t="s">
-        <v>78</v>
+        <v>1360</v>
       </c>
       <c r="C35" t="s">
         <v>189</v>
@@ -8429,7 +8520,7 @@
         <v>43</v>
       </c>
       <c r="B36" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C36" t="s">
         <v>183</v>
@@ -8488,7 +8579,7 @@
         <v>43</v>
       </c>
       <c r="B37" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C37" t="s">
         <v>183</v>
@@ -8547,7 +8638,7 @@
         <v>43</v>
       </c>
       <c r="B38" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C38" t="s">
         <v>183</v>
@@ -8606,7 +8697,7 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C39" t="s">
         <v>183</v>
@@ -8665,7 +8756,7 @@
         <v>43</v>
       </c>
       <c r="B40" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C40" t="s">
         <v>183</v>
@@ -8724,7 +8815,7 @@
         <v>43</v>
       </c>
       <c r="B41" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C41" t="s">
         <v>183</v>
@@ -8783,7 +8874,7 @@
         <v>43</v>
       </c>
       <c r="B42" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C42" t="s">
         <v>183</v>
@@ -8842,7 +8933,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C43" t="s">
         <v>183</v>
@@ -8901,7 +8992,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>74</v>
+        <v>1360</v>
       </c>
       <c r="C44" t="s">
         <v>183</v>
@@ -8960,7 +9051,7 @@
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C45" t="s">
         <v>172</v>
@@ -9019,7 +9110,7 @@
         <v>43</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C46" t="s">
         <v>172</v>
@@ -9078,7 +9169,7 @@
         <v>43</v>
       </c>
       <c r="B47" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C47" t="s">
         <v>172</v>
@@ -9137,7 +9228,7 @@
         <v>43</v>
       </c>
       <c r="B48" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C48" t="s">
         <v>172</v>
@@ -9196,7 +9287,7 @@
         <v>43</v>
       </c>
       <c r="B49" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C49" t="s">
         <v>172</v>
@@ -9255,7 +9346,7 @@
         <v>43</v>
       </c>
       <c r="B50" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C50" t="s">
         <v>172</v>
@@ -9314,7 +9405,7 @@
         <v>43</v>
       </c>
       <c r="B51" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C51" t="s">
         <v>172</v>
@@ -9373,7 +9464,7 @@
         <v>43</v>
       </c>
       <c r="B52" t="s">
-        <v>70</v>
+        <v>1360</v>
       </c>
       <c r="C52" t="s">
         <v>172</v>
@@ -9432,7 +9523,7 @@
         <v>43</v>
       </c>
       <c r="B53" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C53" t="s">
         <v>186</v>
@@ -9491,7 +9582,7 @@
         <v>43</v>
       </c>
       <c r="B54" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C54" t="s">
         <v>186</v>
@@ -9550,7 +9641,7 @@
         <v>43</v>
       </c>
       <c r="B55" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C55" t="s">
         <v>186</v>
@@ -9609,7 +9700,7 @@
         <v>43</v>
       </c>
       <c r="B56" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C56" t="s">
         <v>186</v>
@@ -9668,7 +9759,7 @@
         <v>43</v>
       </c>
       <c r="B57" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C57" t="s">
         <v>186</v>
@@ -9727,7 +9818,7 @@
         <v>43</v>
       </c>
       <c r="B58" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C58" t="s">
         <v>186</v>
@@ -9786,7 +9877,7 @@
         <v>43</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>1360</v>
       </c>
       <c r="C59" t="s">
         <v>186</v>
@@ -9841,7 +9932,7 @@
       </c>
     </row>
   </sheetData>
-  <sortState ref="A4:CT59">
+  <sortState ref="A4:CU59">
     <sortCondition ref="B4:B59"/>
     <sortCondition ref="I4:I59"/>
   </sortState>
@@ -10094,7 +10185,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BU3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="V1" workbookViewId="0">
+    <sheetView topLeftCell="V1" workbookViewId="0">
       <selection activeCell="AI1" sqref="AI1:AK1"/>
     </sheetView>
   </sheetViews>

</xml_diff>